<commit_message>
Actualización a versión 1.3.8.3 - Mejoras de interfaz y correcciones
</commit_message>
<xml_diff>
--- a/data/observaciones.xlsx
+++ b/data/observaciones.xlsx
@@ -525,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,6 +605,90 @@
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>19:38:38</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>LÍNEA 1</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>MÁQUINA 31 T12</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>[General] Comentario</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>19:43:18</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>LÍNEA 3</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>MÁQUINA 33 T16</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>[General] hola</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>19:56:23</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>LÍNEA 2</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>MÁQUINA 32 T23</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>[General] aa</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>admin</t>
         </is>

</xml_diff>

<commit_message>
v1.3.8.4 - Corregidos errores de colores y maximización forzada de lista completa
</commit_message>
<xml_diff>
--- a/data/observaciones.xlsx
+++ b/data/observaciones.xlsx
@@ -13,6 +13,7 @@
     <sheet name="17-08-2025" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="14-12-2025" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="30-08-2025" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="11-08-2025" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -434,13 +435,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
@@ -525,13 +526,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
@@ -689,6 +690,36 @@
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>23:04</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>LÍNEA 2</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>MÁQUINA 29 T8</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>[General] a</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
@@ -711,7 +742,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
@@ -780,7 +811,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
@@ -849,7 +880,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
@@ -918,7 +949,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
@@ -973,4 +1004,93 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Hora</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Línea</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Máquina</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Observación</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Usuario</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>23:21</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>LÍNEA 2</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>MÁQUINA 28 T12</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>[General] aaa</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>